<commit_message>
All elements persisted and Error file created with all elements
</commit_message>
<xml_diff>
--- a/service-order-processor/src/test/data/service_order/201704131155_DataFormatOnly_Batch1_002.xlsx
+++ b/service-order-processor/src/test/data/service_order/201704131155_DataFormatOnly_Batch1_002.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Input" sheetId="1" r:id="rId1"/>
+    <sheet name="Input (2)" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="188">
   <si>
     <t>ActionCode</t>
   </si>
@@ -240,9 +240,6 @@
     <t>Fail - No StartDate</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Fail - Invalid Start Date</t>
   </si>
   <si>
@@ -583,6 +580,9 @@
   </si>
   <si>
     <t>01493660699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pass </t>
   </si>
 </sst>
 </file>
@@ -908,7 +908,7 @@
   <dimension ref="A1:AP32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,7 +1229,7 @@
         <v>67</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>43</v>
@@ -1255,28 +1255,28 @@
         <v>36526</v>
       </c>
       <c r="R3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="U3" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="T3" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="X3" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="AP3" t="s">
-        <v>62</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1324,25 +1324,25 @@
         <v>36526</v>
       </c>
       <c r="R4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="U4" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="T4" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="AP4" t="s">
         <v>62</v>
@@ -1393,25 +1393,25 @@
         <v>36526</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="U5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V5" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V5" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="W5" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AP5" t="s">
         <v>63</v>
@@ -1436,7 +1436,7 @@
         <v>67</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>43</v>
@@ -1462,25 +1462,25 @@
         <v>36526</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="U6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V6" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V6" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="W6" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X6" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AP6" t="s">
         <v>64</v>
@@ -1505,7 +1505,7 @@
         <v>67</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>43</v>
@@ -1531,25 +1531,25 @@
         <v>36526</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="U7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V7" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V7" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="W7" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AP7" t="s">
         <v>65</v>
@@ -1574,7 +1574,7 @@
         <v>67</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>43</v>
@@ -1600,25 +1600,25 @@
         <v>36526</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="U8" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V8" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V8" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="W8" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="X8" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AP8" t="s">
         <v>66</v>
@@ -1643,7 +1643,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>43</v>
@@ -1669,25 +1669,25 @@
         <v>36526</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U9" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V9" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V9" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="W9" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="X9" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AP9" t="s">
         <v>68</v>
@@ -1738,25 +1738,25 @@
         <v>36526</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V10" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V10" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="W10" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AP10" t="s">
         <v>69</v>
@@ -1783,7 +1783,7 @@
         <v>67</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="4" t="s">
@@ -1807,25 +1807,25 @@
         <v>36526</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U11" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V11" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V11" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="W11" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="X11" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AP11" t="s">
         <v>70</v>
@@ -1852,7 +1852,7 @@
         <v>67</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>43</v>
@@ -1876,25 +1876,25 @@
         <v>36526</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="U12" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V12" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V12" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="W12" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="X12" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AP12" t="s">
         <v>71</v>
@@ -1921,7 +1921,7 @@
         <v>67</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>43</v>
@@ -1945,25 +1945,25 @@
         <v>36526</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="U13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V13" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V13" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="W13" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="X13" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AP13" t="s">
         <v>72</v>
@@ -1990,7 +1990,7 @@
         <v>67</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>43</v>
@@ -1999,9 +1999,7 @@
         <v>53</v>
       </c>
       <c r="K14" s="3"/>
-      <c r="L14" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="L14" s="5"/>
       <c r="M14" s="3"/>
       <c r="N14" s="5">
         <v>36526</v>
@@ -2016,28 +2014,28 @@
         <v>36526</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U14" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V14" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V14" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="W14" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="X14" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AP14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2061,7 +2059,7 @@
         <v>67</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>43</v>
@@ -2074,43 +2072,43 @@
         <v>36526</v>
       </c>
       <c r="M15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="N15" s="5">
+        <v>36526</v>
+      </c>
+      <c r="O15" s="5">
+        <v>36526</v>
+      </c>
+      <c r="P15" s="5">
+        <v>36526</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>36526</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="W15" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="X15" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AP15" t="s">
         <v>75</v>
-      </c>
-      <c r="N15" s="5">
-        <v>36526</v>
-      </c>
-      <c r="O15" s="5">
-        <v>36526</v>
-      </c>
-      <c r="P15" s="5">
-        <v>36526</v>
-      </c>
-      <c r="Q15" s="5">
-        <v>36526</v>
-      </c>
-      <c r="R15" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="S15" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="T15" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="U15" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="V15" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="W15" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="X15" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="AP15" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2134,7 +2132,7 @@
         <v>67</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>43</v>
@@ -2160,28 +2158,28 @@
         <v>36526</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U16" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V16" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V16" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="W16" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="X16" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AP16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2205,7 +2203,7 @@
         <v>67</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>43</v>
@@ -2231,28 +2229,28 @@
         <v>36526</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T17" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U17" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V17" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V17" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="W17" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X17" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AP17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2276,7 +2274,7 @@
         <v>67</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>43</v>
@@ -2302,28 +2300,28 @@
         <v>36526</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T18" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="U18" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V18" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V18" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="W18" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X18" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AP18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2347,7 +2345,7 @@
         <v>67</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>43</v>
@@ -2373,28 +2371,28 @@
         <v>36526</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="T19" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="U19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V19" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V19" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="W19" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X19" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AP19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2418,7 +2416,7 @@
         <v>67</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>43</v>
@@ -2444,25 +2442,25 @@
         <v>36526</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T20" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U20" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V20" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V20" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="W20" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X20" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AP20" t="s">
         <v>55</v>
@@ -2489,7 +2487,7 @@
         <v>67</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>43</v>
@@ -2515,28 +2513,28 @@
         <v>36526</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U21" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V21" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V21" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="W21" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="X21" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AP21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2560,7 +2558,7 @@
         <v>67</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>43</v>
@@ -2573,7 +2571,7 @@
         <v>36526</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N22" s="5">
         <v>36526</v>
@@ -2588,25 +2586,25 @@
         <v>36526</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="T22" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U22" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V22" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V22" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="W22" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="X22" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AP22" t="s">
         <v>55</v>
@@ -2633,7 +2631,7 @@
         <v>67</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>43</v>
@@ -2646,7 +2644,7 @@
         <v>36557</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N23" s="5">
         <v>36526</v>
@@ -2661,25 +2659,25 @@
         <v>36526</v>
       </c>
       <c r="R23" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="S23" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="S23" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="T23" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U23" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V23" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="W23" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="X23" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AP23" t="s">
         <v>55</v>
@@ -2706,7 +2704,7 @@
         <v>67</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>43</v>
@@ -2732,25 +2730,25 @@
         <v>36526</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="T24" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="U24" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V24" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="W24" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="X24" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AP24" t="s">
         <v>55</v>
@@ -2805,25 +2803,25 @@
         <v>40689</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="T25" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="U25" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V25" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="W25" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X25" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AP25" t="s">
         <v>57</v>
@@ -2878,25 +2876,25 @@
         <v>40689</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S26" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="T26" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="U26" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V26" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="W26" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="X26" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AP26" t="s">
         <v>58</v>
@@ -2949,25 +2947,25 @@
         <v>40394</v>
       </c>
       <c r="R27" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="S27" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T27" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="U27" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V27" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="W27" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="X27" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AP27" t="s">
         <v>60</v>
@@ -3020,25 +3018,25 @@
         <v>39939</v>
       </c>
       <c r="R28" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="T28" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="U28" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V28" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W28" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="X28" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AP28" t="s">
         <v>55</v>
@@ -3091,25 +3089,25 @@
         <v>40323</v>
       </c>
       <c r="R29" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S29" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T29" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="U29" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V29" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W29" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="X29" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AP29" t="s">
         <v>55</v>

</xml_diff>